<commit_message>
Updated notes for DEQ IR #204435
</commit_message>
<xml_diff>
--- a/incident_history/table/raap_incident_table_2018_sep2021.xlsx
+++ b/incident_history/table/raap_incident_table_2018_sep2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tweiglein/Documents/Graduate School/Virginia Tech - Ph.D./IGC IGEP/RAAP/RAAP_transparency_project/incident_history/table/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32CFE192-E636-7244-8DC7-1F32D400A2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E311D7-42B6-104E-BE7F-C1A859CDC5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -154,9 +154,6 @@
     <t>https://portal.deq.virginia.gov/prep/Report/Details?Id=204435</t>
   </si>
   <si>
-    <t>Nitroglycerin concentration from Original Call Material Description</t>
-  </si>
-  <si>
     <t>Brine water</t>
   </si>
   <si>
@@ -299,6 +296,9 @@
   </si>
   <si>
     <t>https://portal.deq.virginia.gov/prep/Report/Details?Id=300834</t>
+  </si>
+  <si>
+    <t>Nitroglycerin concentration from NRC original call description</t>
   </si>
 </sst>
 </file>
@@ -356,6 +356,7 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -626,9 +627,9 @@
   </sheetPr>
   <dimension ref="A1:O973"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
+      <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -642,43 +643,43 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="O1" s="1"/>
     </row>
@@ -1303,7 +1304,7 @@
         <v>3</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1317,7 +1318,7 @@
         <v>43595</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E18" s="8">
         <v>15</v>
@@ -1329,7 +1330,7 @@
         <v>205978</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>5</v>
@@ -1379,10 +1380,10 @@
         <v>43622</v>
       </c>
       <c r="L19" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="M19" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="M19" s="6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1396,7 +1397,7 @@
         <v>43654</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>3</v>
@@ -1408,7 +1409,7 @@
         <v>291484</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>5</v>
@@ -1423,7 +1424,7 @@
         <v>3</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1449,7 +1450,7 @@
         <v>291447</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>5</v>
@@ -1475,7 +1476,7 @@
         <v>43699</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E22" s="11">
         <v>110</v>
@@ -1487,7 +1488,7 @@
         <v>291894</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>22</v>
@@ -1513,7 +1514,7 @@
         <v>43720</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>3</v>
@@ -1525,7 +1526,7 @@
         <v>292110</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>5</v>
@@ -1551,7 +1552,7 @@
         <v>43724</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E24" s="11">
         <v>161</v>
@@ -1563,7 +1564,7 @@
         <v>292120</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>22</v>
@@ -1601,7 +1602,7 @@
         <v>292468</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>5</v>
@@ -1639,7 +1640,7 @@
         <v>293289</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>5</v>
@@ -1677,7 +1678,7 @@
         <v>293731</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>5</v>
@@ -1715,7 +1716,7 @@
         <v>297147</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>5</v>
@@ -1741,7 +1742,7 @@
         <v>44146</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E29" s="11">
         <v>1000</v>
@@ -1753,7 +1754,7 @@
         <v>297367</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I29" s="6" t="s">
         <v>5</v>
@@ -1779,7 +1780,7 @@
         <v>44193</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E30" s="11">
         <v>2300</v>
@@ -1791,7 +1792,7 @@
         <v>297843</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I30" s="6" t="s">
         <v>5</v>
@@ -1803,7 +1804,7 @@
         <v>44231</v>
       </c>
       <c r="L30" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1817,7 +1818,7 @@
         <v>44284</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E31" s="11">
         <v>800</v>
@@ -1829,7 +1830,7 @@
         <v>298953</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I31" s="6" t="s">
         <v>22</v>
@@ -1841,10 +1842,10 @@
         <v>44329</v>
       </c>
       <c r="L31" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="M31" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1870,7 +1871,7 @@
         <v>299626</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>5</v>
@@ -1896,7 +1897,7 @@
         <v>44362</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E33" s="8">
         <v>2000</v>
@@ -1908,7 +1909,7 @@
         <v>299872</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I33" s="6" t="s">
         <v>22</v>
@@ -1934,7 +1935,7 @@
         <v>44410</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E34" s="8">
         <v>30</v>
@@ -1946,7 +1947,7 @@
         <v>300408</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I34" s="6" t="s">
         <v>22</v>
@@ -1972,7 +1973,7 @@
         <v>44418</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E35" s="4">
         <v>500</v>
@@ -1984,7 +1985,7 @@
         <v>300834</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I35" s="10" t="s">
         <v>5</v>
@@ -2010,7 +2011,7 @@
         <v>44461</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>3</v>
@@ -2022,7 +2023,7 @@
         <v>300963</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I36" s="10" t="s">
         <v>5</v>

</xml_diff>